<commit_message>
Made new result spreadsheets
</commit_message>
<xml_diff>
--- a/Current_Workspace/testOutput.xlsx
+++ b/Current_Workspace/testOutput.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan.c.larson\Documents\GitHub\SMART_UAV_disaster_algorithm_1\Current_Workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704242FC-5EB5-422E-9711-1305E83189F0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BC515A-4EA6-4293-AE62-58E9C5705B58}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11352" windowHeight="11220" activeTab="1" xr2:uid="{3F5B97A5-B34E-4C9D-A5E0-4127B59BC127}"/>
   </bookViews>

</xml_diff>